<commit_message>
First draft of H5G.
</commit_message>
<xml_diff>
--- a/doc/HDF.PInvoke.xlsx
+++ b/doc/HDF.PInvoke.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23955" windowHeight="13110" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23955" windowHeight="13110"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="16" r:id="rId1"/>
@@ -2782,11 +2782,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="186368000"/>
-        <c:axId val="186369536"/>
+        <c:axId val="187219968"/>
+        <c:axId val="187221504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186368000"/>
+        <c:axId val="187219968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,7 +2795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186369536"/>
+        <c:crossAx val="187221504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2803,7 +2803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186369536"/>
+        <c:axId val="187221504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2833,7 +2833,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186368000"/>
+        <c:crossAx val="187219968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3333,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,7 +3587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3729,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B175"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>